<commit_message>
Half of first part
</commit_message>
<xml_diff>
--- a/fin/fins.xlsx
+++ b/fin/fins.xlsx
@@ -374,7 +374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,251 +406,6 @@
       </c>
       <c r="T1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20">
-      <c r="A33" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20">
-      <c r="A34" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20">
-      <c r="A35" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20">
-      <c r="A36" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20">
-      <c r="A37" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20">
-      <c r="A38" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20">
-      <c r="A39" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20">
-      <c r="A40" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20">
-      <c r="A41" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20">
-      <c r="A42" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20">
-      <c r="A43" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20">
-      <c r="A44" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20">
-      <c r="A45" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20">
-      <c r="A46" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20">
-      <c r="A47" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20">
-      <c r="A48" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20">
-      <c r="A49" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20">
-      <c r="A50" t="n">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving on to notebook
</commit_message>
<xml_diff>
--- a/fin/fins.xlsx
+++ b/fin/fins.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Days</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Sunday</t>
+  </si>
+  <si>
+    <t>Date\Type</t>
   </si>
 </sst>
 </file>
@@ -374,13 +377,35 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="13.2"/>
+    <col customWidth="1" max="2" min="2" width="9.6"/>
+    <col customWidth="1" max="3" min="3" width="2.4"/>
+    <col customWidth="1" max="4" min="4" width="2.4"/>
+    <col customWidth="1" max="5" min="5" width="10.8"/>
+    <col customWidth="1" max="6" min="6" width="2.4"/>
+    <col customWidth="1" max="7" min="7" width="2.4"/>
+    <col customWidth="1" max="8" min="8" width="13.2"/>
+    <col customWidth="1" max="9" min="9" width="2.4"/>
+    <col customWidth="1" max="10" min="10" width="2.4"/>
+    <col customWidth="1" max="11" min="11" width="12"/>
+    <col customWidth="1" max="12" min="12" width="2.4"/>
+    <col customWidth="1" max="13" min="13" width="2.4"/>
+    <col customWidth="1" max="14" min="14" width="9.6"/>
+    <col customWidth="1" max="15" min="15" width="2.4"/>
+    <col customWidth="1" max="16" min="16" width="2.4"/>
+    <col customWidth="1" max="17" min="17" width="12"/>
+    <col customWidth="1" max="18" min="18" width="2.4"/>
+    <col customWidth="1" max="19" min="19" width="2.4"/>
+    <col customWidth="1" max="20" min="20" width="9.6"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
@@ -406,6 +431,11 @@
       </c>
       <c r="T1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One step closer to the end
</commit_message>
<xml_diff>
--- a/fin/fins.xlsx
+++ b/fin/fins.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="M1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="V9" xSplit="0" ySplit="2"/>
@@ -2081,18 +2081,54 @@
         <f>SUM(F41:F43)</f>
         <v/>
       </c>
-      <c r="K41" t="inlineStr">
+      <c r="K41" s="18" t="inlineStr">
         <is>
           <t>milk</t>
         </is>
       </c>
-      <c r="L41" t="n">
+      <c r="L41" s="18" t="n">
         <v>150</v>
       </c>
       <c r="M41" s="28">
         <f>SUM(L41:L43)</f>
         <v/>
       </c>
+      <c r="N41" s="18" t="inlineStr">
+        <is>
+          <t>chill</t>
+        </is>
+      </c>
+      <c r="O41" s="18" t="n">
+        <v>150</v>
+      </c>
+      <c r="P41" s="28">
+        <f>SUM(O41:O42)</f>
+        <v/>
+      </c>
+      <c r="Q41" s="18" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="R41" s="18" t="n">
+        <v>104</v>
+      </c>
+      <c r="S41" s="28">
+        <f>SUM(R41:R41)</f>
+        <v/>
+      </c>
+      <c r="T41" s="18" t="inlineStr">
+        <is>
+          <t>chill</t>
+        </is>
+      </c>
+      <c r="U41" s="18" t="n">
+        <v>80</v>
+      </c>
+      <c r="V41" s="28">
+        <f>SUM(U41:U41)</f>
+        <v/>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="18" t="inlineStr">
@@ -2116,13 +2152,21 @@
       <c r="F42" s="18" t="n">
         <v>42</v>
       </c>
-      <c r="K42" t="inlineStr">
+      <c r="K42" s="18" t="inlineStr">
         <is>
           <t>bananas</t>
         </is>
       </c>
-      <c r="L42" t="n">
+      <c r="L42" s="18" t="n">
         <v>75</v>
+      </c>
+      <c r="N42" s="18" t="inlineStr">
+        <is>
+          <t>dinned</t>
+        </is>
+      </c>
+      <c r="O42" s="18" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="43">
@@ -2147,12 +2191,12 @@
       <c r="F43" s="18" t="n">
         <v>180</v>
       </c>
-      <c r="K43" t="inlineStr">
+      <c r="K43" s="18" t="inlineStr">
         <is>
           <t>dinner</t>
         </is>
       </c>
-      <c r="L43" t="n">
+      <c r="L43" s="18" t="n">
         <v>55</v>
       </c>
     </row>
@@ -2186,9 +2230,218 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46"/>
+    <row r="46">
+      <c r="A46" s="18" t="inlineStr">
+        <is>
+          <t>1/4/2019</t>
+        </is>
+      </c>
+      <c r="B46" s="18" t="inlineStr">
+        <is>
+          <t>dinner</t>
+        </is>
+      </c>
+      <c r="C46" s="18" t="n">
+        <v>55</v>
+      </c>
+      <c r="D46" s="28">
+        <f>SUM(C46:C50)</f>
+        <v/>
+      </c>
+      <c r="E46" s="18" t="inlineStr">
+        <is>
+          <t>dinner</t>
+        </is>
+      </c>
+      <c r="F46" s="18" t="n">
+        <v>215</v>
+      </c>
+      <c r="G46" s="28">
+        <f>SUM(F46:F52)</f>
+        <v/>
+      </c>
+      <c r="H46" s="18" t="inlineStr">
+        <is>
+          <t>snacks</t>
+        </is>
+      </c>
+      <c r="I46" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="J46" s="28">
+        <f>SUM(I46:I48)</f>
+        <v/>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>dinner</t>
+        </is>
+      </c>
+      <c r="L46" t="n">
+        <v>180</v>
+      </c>
+      <c r="M46" s="28">
+        <f>SUM(L46:L48)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="B47" s="18" t="inlineStr">
+        <is>
+          <t>metro</t>
+        </is>
+      </c>
+      <c r="C47" s="18" t="n">
+        <v>395</v>
+      </c>
+      <c r="E47" s="18" t="inlineStr">
+        <is>
+          <t>bananas</t>
+        </is>
+      </c>
+      <c r="F47" s="18" t="n">
+        <v>17</v>
+      </c>
+      <c r="H47" s="18" t="inlineStr">
+        <is>
+          <t>en. drink</t>
+        </is>
+      </c>
+      <c r="I47" s="18" t="n">
+        <v>120</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L47" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="B48" s="18" t="inlineStr">
+        <is>
+          <t>breakfast</t>
+        </is>
+      </c>
+      <c r="C48" s="18" t="n">
+        <v>110</v>
+      </c>
+      <c r="E48" s="18" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="F48" s="18" t="n">
+        <v>22</v>
+      </c>
+      <c r="H48" s="18" t="inlineStr">
+        <is>
+          <t>hygiene</t>
+        </is>
+      </c>
+      <c r="I48" s="18" t="n">
+        <v>30</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="L48" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="B49" s="18" t="inlineStr">
+        <is>
+          <t>hygiene</t>
+        </is>
+      </c>
+      <c r="C49" s="18" t="n">
+        <v>165</v>
+      </c>
+      <c r="E49" s="18" t="inlineStr">
+        <is>
+          <t>salmon</t>
+        </is>
+      </c>
+      <c r="F49" s="18" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="B50" s="18" t="inlineStr">
+        <is>
+          <t>bananas</t>
+        </is>
+      </c>
+      <c r="C50" s="18" t="n">
+        <v>70</v>
+      </c>
+      <c r="E50" s="18" t="inlineStr">
+        <is>
+          <t>bread</t>
+        </is>
+      </c>
+      <c r="F50" s="18" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="E51" s="18" t="inlineStr">
+        <is>
+          <t>garlic</t>
+        </is>
+      </c>
+      <c r="F51" s="18" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="E52" s="18" t="inlineStr">
+        <is>
+          <t>blueberries</t>
+        </is>
+      </c>
+      <c r="F52" s="18" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53"/>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="56">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
@@ -2238,6 +2491,13 @@
     <mergeCell ref="D41:D45"/>
     <mergeCell ref="G41:G43"/>
     <mergeCell ref="M41:M43"/>
+    <mergeCell ref="P41:P42"/>
+    <mergeCell ref="S41"/>
+    <mergeCell ref="V41"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="G46:G52"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="M46:M48"/>
   </mergeCells>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>

</xml_diff>